<commit_message>
Afegits a la base de dades de la llibreria i similars tots els commits anteriors: DLW5BT, connector M8, STM32L011D3P6, ST3485ECDR
</commit_message>
<xml_diff>
--- a/Library/CSE_LIB.xlsx
+++ b/Library/CSE_LIB.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOCALPRJ\PCB\CSE_AltiumLib\Library\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="676" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="676" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Resistencies" sheetId="1" r:id="rId1"/>
@@ -33,19 +38,19 @@
     <sheet name="Control" sheetId="24" r:id="rId24"/>
   </sheets>
   <definedNames>
+    <definedName name="__xlfn_BAHTTEXT">NA()</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Condensadors No Polaritzats'!$A$1:$AF$94</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Inductius!$A$1:$AG$107</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Microcontroladors!$A$1:$AH$246</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resistencies!$A$1:$S$791</definedName>
-    <definedName name="__xlfn_BAHTTEXT">NA()</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'Logica no programable i generic'!$A$1:$O$21</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="17">Optiques!$A$1:$R$30</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="1">'Condensadors No Polaritzats'!$A$1:$R$172</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="2">'Condensadors Polaritzats'!$A$2:$Q$250</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="4">Microcontroladors!$A$1:$AH$241</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Logica no programable i generic'!$A$1:$O$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="17">Optiques!$A$1:$R$30</definedName>
     <definedName name="TMPPRTS">'Logica Programable'!$A$1:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -55,7 +60,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21342" uniqueCount="5360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21355" uniqueCount="5365">
   <si>
     <t>Part Number</t>
   </si>
@@ -16196,6 +16201,21 @@
   </si>
   <si>
     <t>QFN50P500X500-28W1L</t>
+  </si>
+  <si>
+    <t>STM32L011D3P6</t>
+  </si>
+  <si>
+    <t>Cortex M0+ Low Power</t>
+  </si>
+  <si>
+    <t>1V65-3V6</t>
+  </si>
+  <si>
+    <t>8k</t>
+  </si>
+  <si>
+    <t>TSOP65P640-14AL</t>
   </si>
 </sst>
 </file>
@@ -16440,7 +16460,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -16448,6 +16468,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -16833,37 +16856,37 @@
       <selection pane="bottomLeft" activeCell="L984" sqref="L984"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="20" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="54.6640625" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="54.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" customWidth="1"/>
-    <col min="26" max="26" width="15.88671875" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1"/>
     <col min="27" max="27" width="14" customWidth="1"/>
-    <col min="28" max="28" width="16.6640625" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="32" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -49521,21 +49544,21 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" customWidth="1"/>
-    <col min="6" max="6" width="59.21875" customWidth="1"/>
-    <col min="7" max="7" width="37.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="45.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" customWidth="1"/>
-    <col min="16" max="18" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="59.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="45.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="16" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -50212,31 +50235,31 @@
       <selection pane="bottomLeft" activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15" style="38" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="38" customWidth="1"/>
     <col min="4" max="4" width="15" style="38" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="38" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="38" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="38"/>
-    <col min="9" max="9" width="67.5546875" style="38" customWidth="1"/>
-    <col min="10" max="10" width="37.77734375" style="38" customWidth="1"/>
-    <col min="11" max="11" width="21.21875" style="38" customWidth="1"/>
-    <col min="12" max="12" width="47.77734375" style="38" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" style="38" customWidth="1"/>
-    <col min="14" max="15" width="11.109375" style="38"/>
-    <col min="16" max="17" width="13.44140625" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.109375" style="38"/>
-    <col min="19" max="19" width="15.6640625" style="38" customWidth="1"/>
-    <col min="20" max="20" width="94.6640625" style="38" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" style="38" customWidth="1"/>
-    <col min="22" max="16384" width="11.109375" style="38"/>
+    <col min="5" max="5" width="7.140625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="38" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="38"/>
+    <col min="9" max="9" width="67.5703125" style="38" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" style="38" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="38" customWidth="1"/>
+    <col min="12" max="12" width="47.7109375" style="38" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="38" customWidth="1"/>
+    <col min="14" max="15" width="11.140625" style="38"/>
+    <col min="16" max="17" width="13.42578125" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="38"/>
+    <col min="19" max="19" width="15.7109375" style="38" customWidth="1"/>
+    <col min="20" max="20" width="94.7109375" style="38" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="38" customWidth="1"/>
+    <col min="22" max="16384" width="11.140625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="39.6">
+    <row r="1" spans="1:33" ht="38.25">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -52086,23 +52109,23 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="95.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="95.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-    <col min="9" max="9" width="23.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
-    <col min="13" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="67.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="13" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.6">
+    <row r="1" spans="1:30" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -52517,24 +52540,24 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="71.21875" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="71.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="39.6">
+    <row r="1" spans="1:29" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -52699,22 +52722,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="14" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="98.5546875" customWidth="1"/>
+    <col min="14" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="98.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="39.6">
+    <row r="1" spans="1:29" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -52838,30 +52861,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="63.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="32.77734375" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
-    <col min="10" max="10" width="23.77734375" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" customWidth="1"/>
     <col min="18" max="18" width="21" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="207.21875" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="207.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="39.6">
+    <row r="1" spans="1:33" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -53266,23 +53289,23 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="84.5546875" customWidth="1"/>
-    <col min="6" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="32.77734375" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="18" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="84.5703125" customWidth="1"/>
+    <col min="6" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="39.6">
+    <row r="1" spans="1:31" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -53624,25 +53647,25 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="79.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="21.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="20" width="10.6640625" customWidth="1"/>
-    <col min="21" max="23" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="79.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="23" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="39.6">
+    <row r="1" spans="1:36" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -54329,11 +54352,11 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="8" max="8" width="82.6640625" customWidth="1"/>
-    <col min="9" max="9" width="37.77734375" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="8" max="8" width="82.7109375" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -54652,7 +54675,7 @@
         <v>5012</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="14.4">
+    <row r="8" spans="1:32" ht="14.25">
       <c r="A8" s="48" t="s">
         <v>5017</v>
       </c>
@@ -54697,22 +54720,22 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="45.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" customWidth="1"/>
-    <col min="15" max="16" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="15" max="16" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.6">
+    <row r="1" spans="1:30" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -54841,7 +54864,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="26.4">
+    <row r="4" spans="1:30" ht="25.5">
       <c r="A4" t="s">
         <v>5030</v>
       </c>
@@ -54865,7 +54888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="39.6">
+    <row r="5" spans="1:30" ht="38.25">
       <c r="A5" t="s">
         <v>5034</v>
       </c>
@@ -55007,38 +55030,38 @@
       <selection pane="bottomLeft" activeCell="L118" sqref="L118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" style="12" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" customWidth="1"/>
-    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" customWidth="1"/>
     <col min="19" max="19" width="42" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" customWidth="1"/>
-    <col min="26" max="26" width="15.88671875" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1"/>
     <col min="27" max="27" width="14" customWidth="1"/>
-    <col min="28" max="28" width="16.6640625" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="32" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" customWidth="1"/>
+    <col min="30" max="32" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -59620,24 +59643,24 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="44.44140625" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.77734375" customWidth="1"/>
-    <col min="12" max="12" width="20.77734375" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" customWidth="1"/>
-    <col min="19" max="19" width="53.88671875" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="53.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="39.6">
+    <row r="1" spans="1:32" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -59950,31 +59973,31 @@
       <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" customWidth="1"/>
-    <col min="12" max="12" width="7.77734375" customWidth="1"/>
-    <col min="15" max="15" width="69.77734375" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" customWidth="1"/>
-    <col min="18" max="18" width="23.77734375" customWidth="1"/>
-    <col min="24" max="24" width="15.109375" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" customWidth="1"/>
-    <col min="26" max="26" width="71.6640625" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="69.7109375" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" customWidth="1"/>
+    <col min="26" max="26" width="71.7109375" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="39.6">
+    <row r="1" spans="1:39" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -62672,24 +62695,24 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="37.77734375" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="62.5546875" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="62.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.6">
+    <row r="1" spans="1:30" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -63077,22 +63100,22 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="4" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="75.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="23.77734375" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" customWidth="1"/>
-    <col min="18" max="18" width="103.5546875" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="75.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="103.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="39.6">
+    <row r="1" spans="1:31" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -63290,17 +63313,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="5" max="5" width="63.77734375" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39.6">
+    <row r="1" spans="1:30" ht="38.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -63471,37 +63494,37 @@
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="12" width="50.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="50.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="12" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="8.5546875" customWidth="1"/>
-    <col min="17" max="18" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="49.21875" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
-    <col min="22" max="22" width="19.109375" customWidth="1"/>
-    <col min="23" max="23" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="49.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" customWidth="1"/>
+    <col min="23" max="23" width="9.28515625" customWidth="1"/>
     <col min="24" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="17.44140625" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" customWidth="1"/>
-    <col min="27" max="27" width="15.88671875" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
     <col min="28" max="28" width="14" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" customWidth="1"/>
-    <col min="30" max="30" width="13.109375" customWidth="1"/>
-    <col min="31" max="33" width="12.44140625" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" customWidth="1"/>
+    <col min="31" max="33" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -75855,28 +75878,28 @@
       <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="18" customWidth="1"/>
-    <col min="9" max="9" width="65.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="51.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" style="12" customWidth="1"/>
-    <col min="15" max="15" width="11.77734375" style="1" customWidth="1"/>
-    <col min="16" max="17" width="13.44140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="98.33203125" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="65.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="51.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="12" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="1" customWidth="1"/>
+    <col min="16" max="17" width="13.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="98.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -78526,46 +78549,46 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH254"/>
+  <dimension ref="A1:AH255"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A254" sqref="A254"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N255" sqref="N255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="92.109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="21"/>
-    <col min="7" max="7" width="8.77734375" style="21" customWidth="1"/>
-    <col min="8" max="9" width="20.77734375" style="21" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" style="21" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" style="21" customWidth="1"/>
-    <col min="13" max="13" width="47.33203125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="92.140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="8.7109375" style="21" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="21" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="21" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="21" customWidth="1"/>
+    <col min="13" max="13" width="47.28515625" style="21" customWidth="1"/>
     <col min="14" max="14" width="50" style="21" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="22" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" style="21" customWidth="1"/>
-    <col min="17" max="18" width="12.44140625" style="21" customWidth="1"/>
-    <col min="19" max="19" width="27.6640625" style="23" customWidth="1"/>
-    <col min="20" max="20" width="29.6640625" style="23" customWidth="1"/>
-    <col min="21" max="21" width="105.77734375" style="23" customWidth="1"/>
-    <col min="22" max="24" width="9.109375" style="23"/>
-    <col min="25" max="25" width="9.33203125" style="23" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="22" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="21" customWidth="1"/>
+    <col min="17" max="18" width="12.42578125" style="21" customWidth="1"/>
+    <col min="19" max="19" width="27.7109375" style="23" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" style="23" customWidth="1"/>
+    <col min="21" max="21" width="105.7109375" style="23" customWidth="1"/>
+    <col min="22" max="24" width="9.140625" style="23"/>
+    <col min="25" max="25" width="9.28515625" style="23" customWidth="1"/>
     <col min="26" max="26" width="16" style="23" customWidth="1"/>
-    <col min="27" max="27" width="10.88671875" style="23" customWidth="1"/>
-    <col min="28" max="28" width="15.109375" style="23" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" style="23" customWidth="1"/>
-    <col min="30" max="30" width="15.5546875" style="23" customWidth="1"/>
-    <col min="31" max="31" width="12.33203125" style="23" customWidth="1"/>
-    <col min="32" max="32" width="27.6640625" style="23" customWidth="1"/>
-    <col min="33" max="33" width="29.6640625" style="23" customWidth="1"/>
-    <col min="34" max="34" width="11.21875" style="23" customWidth="1"/>
-    <col min="35" max="16384" width="9.109375" style="23"/>
+    <col min="27" max="27" width="10.85546875" style="23" customWidth="1"/>
+    <col min="28" max="28" width="15.140625" style="23" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" style="23" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" style="23" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" style="23" customWidth="1"/>
+    <col min="32" max="32" width="27.7109375" style="23" customWidth="1"/>
+    <col min="33" max="33" width="29.7109375" style="23" customWidth="1"/>
+    <col min="34" max="34" width="11.28515625" style="23" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -89264,6 +89287,47 @@
       </c>
       <c r="N254" s="21" t="s">
         <v>4295</v>
+      </c>
+    </row>
+    <row r="255" spans="1:17">
+      <c r="A255" s="21" t="s">
+        <v>5360</v>
+      </c>
+      <c r="B255" s="21" t="s">
+        <v>3705</v>
+      </c>
+      <c r="D255" s="21" t="s">
+        <v>5360</v>
+      </c>
+      <c r="E255" s="21" t="s">
+        <v>5361</v>
+      </c>
+      <c r="F255" s="21" t="s">
+        <v>3708</v>
+      </c>
+      <c r="G255" s="21" t="s">
+        <v>5362</v>
+      </c>
+      <c r="H255" s="21" t="s">
+        <v>4253</v>
+      </c>
+      <c r="I255" s="21" t="s">
+        <v>5363</v>
+      </c>
+      <c r="J255" s="21" t="s">
+        <v>4293</v>
+      </c>
+      <c r="K255" s="24" t="s">
+        <v>3712</v>
+      </c>
+      <c r="L255" s="21" t="s">
+        <v>5360</v>
+      </c>
+      <c r="M255" s="21" t="s">
+        <v>4396</v>
+      </c>
+      <c r="N255" s="21" t="s">
+        <v>5364</v>
       </c>
     </row>
   </sheetData>
@@ -89283,15 +89347,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="5" max="5" width="61.44140625" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="26.109375" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="23" customFormat="1">
@@ -89494,23 +89558,23 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="63" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.21875" customWidth="1"/>
-    <col min="24" max="25" width="12.44140625" customWidth="1"/>
-    <col min="26" max="26" width="10.21875" customWidth="1"/>
-    <col min="27" max="27" width="6.109375" customWidth="1"/>
-    <col min="28" max="28" width="57.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="24" max="25" width="12.42578125" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" customWidth="1"/>
+    <col min="27" max="27" width="6.140625" customWidth="1"/>
+    <col min="28" max="28" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
@@ -89671,20 +89735,20 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="84.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="84.5703125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="35.109375" customWidth="1"/>
-    <col min="10" max="10" width="25.109375" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" customWidth="1"/>
-    <col min="14" max="14" width="39.44140625" customWidth="1"/>
-    <col min="16" max="18" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" customWidth="1"/>
+    <col min="16" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -90333,23 +90397,23 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="84.44140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="84.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="26.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="73.44140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="17.88671875" customWidth="1"/>
-    <col min="17" max="18" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="73.42578125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">

</xml_diff>